<commit_message>
Added NER gold standard
</commit_message>
<xml_diff>
--- a/gold_standard/gold/ner_gold.xlsx
+++ b/gold_standard/gold/ner_gold.xlsx
@@ -110,7 +110,7 @@
     </r>
   </si>
   <si>
-    <t>ACFT, DITCH, TREE, LOST CONTROL</t>
+    <t>ACFT; DITCH; TREE; LOST CONTROL</t>
   </si>
   <si>
     <t>19800217031649I</t>
@@ -119,7 +119,7 @@
     <t xml:space="preserve">AFTER TAKEOFF, ENGINE QUIT. WING FUEL TANK SUMPS WERE NOT DRAINED DURING PREFLIGHT BECAUSE THEY WERE FROZEN.       </t>
   </si>
   <si>
-    <t>TAKEOFF, ENGINE, WING, FUEL TANK, SUMPS, PREFLIGHT</t>
+    <t>TAKEOFF; ENGINE; WING; FUEL TANK; SUMPS; PREFLIGHT</t>
   </si>
   <si>
     <t>19790720021329A</t>
@@ -128,7 +128,7 @@
     <t xml:space="preserve">HELICOPTER TOOK OFF WITH SLING LOAD ATTACHED. CRASHED WHEN LOAD WEDGED IN TREES. IMPROPER PREFLIGHT.               </t>
   </si>
   <si>
-    <t>HELICOPTER, SLING LOAD, LOAD, TREES, PREFLIGHT</t>
+    <t>HELICOPTER; SLING LOAD; LOAD; TREES; PREFLIGHT</t>
   </si>
   <si>
     <t>19841214074599I</t>
@@ -160,7 +160,7 @@
     </r>
   </si>
   <si>
-    <t>NOSEWHEEL STEERING, BRAKES, AIRCRAFT, FENCE, CIRCUIT BREAKER, HYDRAULIC PUMP</t>
+    <t>NOSEWHEEL STEERING; BRAKES; AIRCRAFT; FENCE; CIRCUIT BREAKER; HYDRAULIC PUMP</t>
   </si>
   <si>
     <t>19860128014289I</t>
@@ -184,7 +184,7 @@
     </r>
   </si>
   <si>
-    <t>FORWARD CARGO DOOR, AIRCRAFT, OBJECTS, WARNING LIGHT</t>
+    <t>FORWARD CARGO DOOR; AIRCRAFT; OBJECTS; WARNING LIGHT</t>
   </si>
   <si>
     <t>20000215010329A</t>
@@ -193,7 +193,7 @@
     <t xml:space="preserve">(-23) MR. TIMOTHY ALLEN WELLS WAS ACTING AS PILOT IN COMMAND OF A BELL HELICOPTER MODEL BHT-47-G5, N4754R, ENGAGED </t>
   </si>
   <si>
-    <t>MR. TIMOTHY ALLEN WELLS, PILOT, BELL, HELICOPTER, BHT-47-G5, N4754R</t>
+    <t>MR. TIMOTHY ALLEN WELLS; PILOT; BELL; HELICOPTER; BHT-47-G5; N4754R</t>
   </si>
   <si>
     <t>19801116083749I</t>
@@ -217,7 +217,7 @@
     </r>
   </si>
   <si>
-    <t>LANDING, ONE, ENGINE, ICE, AUXILIARY FUEL SYSTEM</t>
+    <t>LANDING; ONE; ENGINE; ICE; AUXILIARY FUEL SYSTEM</t>
   </si>
   <si>
     <t>19850315007389A</t>
@@ -226,7 +226,7 @@
     <t xml:space="preserve">PILOT WAS DESCENDING TO LOWER ALTITUDE DUE TO ICING. LOST CONTROL. ALTIMETER NOT IFR CERTIFIED. ICING FORECAST.    </t>
   </si>
   <si>
-    <t>PILOT, ALTITUDE, ICING, LOST CONTROL, ALTIMETER, ICING</t>
+    <t>PILOT; ALTITUDE; ICING; LOST CONTROL; ALTIMETER; ICING</t>
   </si>
   <si>
     <t>20070630826079I</t>
@@ -235,7 +235,7 @@
     <t>(-23) AIRCRAFT DEPARTED RAY AIRPORT AND AFTER TAKEOFF INTO THE CLIMB AIRCRAFT ENGINE STARTED TO HAVE PROBLEMS. PILO</t>
   </si>
   <si>
-    <t>AIRCRAFT, RAY AIRPORT, TAKEOFF, AIRCRAFT, ENGINE, PROBLEMS</t>
+    <t>AIRCRAFT; RAY AIRPORT; TAKEOFF; AIRCRAFT; ENGINE; PROBLEMS</t>
   </si>
   <si>
     <t>19900425011659A</t>
@@ -244,7 +244,7 @@
     <t xml:space="preserve">RAN OUT OF FUEL ON FERRY FLIGHT. LEFT PONTOON SEPARATED LANDING IN A POND. FUEL CAP NOT SECURED. FUEL SIPHONED.    </t>
   </si>
   <si>
-    <t>FUEL, FERRY FLIGHT, LEFT PONTOON, LANDING, POND, FUEL CAP, FUEL</t>
+    <t>FUEL; FERRY FLIGHT; LEFT PONTOON; LANDING; POND; FUEL CAP; FUEL</t>
   </si>
   <si>
     <t>19991230042089A</t>
@@ -253,7 +253,7 @@
     <t xml:space="preserve">(.4)THE PILOT SAID THAT SHORTLY AFTER TAKEOFF, THE ENGINE 'STARTED CUTTING OUT AND WAS NOT DEVELOPING ENOUGH POWER </t>
   </si>
   <si>
-    <t>PILOT, TAKEOFF, ENGINE, POWER</t>
+    <t>PILOT; TAKEOFF; ENGINE; POWER</t>
   </si>
   <si>
     <t>19820725041999I</t>
@@ -262,7 +262,7 @@
     <t xml:space="preserve">LOOSE COWLING ON TAKEOFF. COWLING CAME OFF ON RETURNING TO LAND. CRACKED WINDSHIELD, DENTED STABILIZER.            </t>
   </si>
   <si>
-    <t>COWLING, TAKEOFF, COWLING, LAND, WINDSHIELD, STABILIZER</t>
+    <t>COWLING; TAKEOFF; COWLING; LAND; WINDSHIELD; STABILIZER</t>
   </si>
   <si>
     <t>19940412011509I</t>
@@ -271,7 +271,7 @@
     <t xml:space="preserve">AIRCRAFT POPPED OPEN ON DESCENT. FLIGHT MANUAL FLEW OUT AND STRUCK TRUCK WINDSHIELD ON GROUND. LANDED SAFELY.      </t>
   </si>
   <si>
-    <t>AIRCRAFT, DESCENT, FLIGHT MANUAL, TRUCK, WINDSHIELD, GROUND</t>
+    <t>AIRCRAFT; DESCENT; FLIGHT MANUAL; TRUCK; WINDSHIELD; GROUND</t>
   </si>
   <si>
     <t>19971226042729I</t>
@@ -280,7 +280,7 @@
     <t>NR2 ENGINE FIRE WHILE LOADING PASSENGERS AT GATE. EVACUATED. FUEL LEVER WAS IN FLIGHT IDLE. CUT OFF. SMOKE CLEARED.</t>
   </si>
   <si>
-    <t>NR2 ENGINE, ENGINE FIRE, PASSENGERS, GATE, FUEL LEVER, SMOKE</t>
+    <t>NR2 ENGINE; ENGINE FIRE; PASSENGERS; GATE; FUEL LEVER; SMOKE</t>
   </si>
   <si>
     <t>19950619021589I</t>
@@ -289,7 +289,7 @@
     <t xml:space="preserve">AFTER DEPARTING HIGH OIL TEMP. LANDED OFF AIRPOR. SHEARED MAIN GEAR. FOUND LOW ON OIL.                             </t>
   </si>
   <si>
-    <t>OIL TEMP, GEAR, OIL</t>
+    <t>OIL TEMP; GEAR; OIL</t>
   </si>
   <si>
     <t>19940815046149I</t>
@@ -298,7 +298,7 @@
     <t xml:space="preserve">BATTERY COMPARTMENT DOOR CAME OPEN. ANTENNA CRACKED WINDSHIELD.                                                    </t>
   </si>
   <si>
-    <t>BATTERY COMPARTMENT DOOR, ANTENNA, WINDSHIELD</t>
+    <t>BATTERY COMPARTMENT DOOR; ANTENNA; WINDSHIELD</t>
   </si>
   <si>
     <t>19860228038269I</t>
@@ -307,7 +307,7 @@
     <t xml:space="preserve">RETURNED WHEN NOSE GEAR FAILED TO RETRACT. FOUND THAT PIN HAD NOT BEEN REMOVED AFTER PREVIOUS MAINTENANCE.         </t>
   </si>
   <si>
-    <t>NOSE GEAR, PIN, MAINTENANCE</t>
+    <t>NOSE GEAR; PIN; MAINTENANCE</t>
   </si>
   <si>
     <t>19790718019229I</t>
@@ -316,7 +316,7 @@
     <t xml:space="preserve">GROUND STAND BAGGAGE CART WITH INOPERATIVE BRAKES ROLLED INTO SIDE OF PARKED AIRCRAFT. 9 INCH TEAR IN FUSELAGE.    </t>
   </si>
   <si>
-    <t>STAND, BAGGAGE CART, BRAKES, AIRCRAFT, TEAR, FUSELAGE</t>
+    <t>STAND; BAGGAGE CART; BRAKES; AIRCRAFT; TEAR; FUSELAGE</t>
   </si>
   <si>
     <t>20000625032189I</t>
@@ -325,7 +325,7 @@
     <t>(-23)NORTHWEST AIRLINES DC-10 BOEING PUSHED BACK FOR REPOSITIONING OFF OF GATE B-52 STRUCK A CONTINENTAL AIRLINES D</t>
   </si>
   <si>
-    <t>NORTHWEST AIRLINES, DC-10, BOEING, GATE B-52, CONTINENTAL AIRLINES</t>
+    <t>NORTHWEST AIRLINES; DC-10; BOEING; GATE B-52; CONTINENTAL AIRLINES</t>
   </si>
   <si>
     <t>19860530030499A</t>
@@ -334,7 +334,7 @@
     <t xml:space="preserve">ENGINE OVERHEAT. HOT OIL SMELL.KNEW HE HAD FAILED TO REMOVE AIR INTAKE PLUGS. NOSED OVER IN FURROWS PLOWED FAILED  </t>
   </si>
   <si>
-    <t>ENGINE, OIL SMELL, AIR INTAKE PLUGS, FURROWS</t>
+    <t>ENGINE; OIL SMELL; AIR INTAKE PLUGS; FURROWS</t>
   </si>
   <si>
     <t>19821117066379I</t>
@@ -343,7 +343,7 @@
     <t>PILOT UNABLE TO PRESSURIZE. FOUND ACCESS DOOR SLIGHTLY OPEN. DEPRESSURIZED. DOOR OPENED FULLY. STOPPED BY FUSELAGE.</t>
   </si>
   <si>
-    <t>PILOT, ACCESS DOOR, DOOR, FUSELAGE</t>
+    <t>PILOT; ACCESS DOOR; DOOR; FUSELAGE</t>
   </si>
   <si>
     <t>19810303007119A</t>
@@ -352,7 +352,7 @@
     <t xml:space="preserve">VEERED OFF RUNWAY ON LANDING.  HIT PARKED AIRPLANE.  NEWLY INSTALLED CARPETING RESTRICTED RUDDER PEDAL MOVEMENT.   </t>
   </si>
   <si>
-    <t>RUNWAY, LANDING, AIRPLANE, CARPETING, RUDDER PEDAL</t>
+    <t>RUNWAY; LANDING; AIRPLANE; CARPETING; RUDDER PEDAL</t>
   </si>
   <si>
     <t>19950602032329I</t>
@@ -361,7 +361,7 @@
     <t xml:space="preserve">VEERED OFF TAXIWAY. STRUCK TAXIWAY LIGHT. WAS ADVISED DAMAGED PROP. CONTINUED TO LIT.                              </t>
   </si>
   <si>
-    <t>TAXIWAY, TAXIWAY LIGHT, PROP</t>
+    <t>TAXIWAY; TAXIWAY LIGHT; PROP</t>
   </si>
   <si>
     <t>19901101064289I</t>
@@ -370,7 +370,7 @@
     <t>FUEL CAP MISSING FROM RIGHT TANK AND GAS ESCAPING WHILE TAXIING. REPLACED CAP. RESUMED FLIGHT WITHOUT CLEANING WING</t>
   </si>
   <si>
-    <t>FUEL CAP, RIGHT TANK, GAS, CAP, FLIGHT, WING</t>
+    <t>FUEL CAP; RIGHT TANK; GAS; CAP; FLIGHT; WING</t>
   </si>
   <si>
     <t>20050713014239I</t>
@@ -379,7 +379,7 @@
     <t xml:space="preserve">(-23) ON JULY 13, 2005, AT 1535 MST, AN RAYTHEON AIRCRAFT CO. B36TC (BONANZA), N3042V REGISTERED TO HAVENS LEASING </t>
   </si>
   <si>
-    <t>JULY 13, 2005, 1535 MST, RAYTHEON AIRCRAFT CO, B36TC, BONANZA, N3042V, HAVENS LEASING</t>
+    <t>JULY 13, 2005; 1535 MST; RAYTHEON AIRCRAFT CO; B36TC; BONANZA; N3042V; HAVENS LEASING</t>
   </si>
   <si>
     <t>19860706034879A</t>
@@ -388,7 +388,7 @@
     <t xml:space="preserve">THE ENGINE LOST POWER ON TAKEOFF AND THE AIRCRAFT FLIPPED ON LANDING.PILOT HAD JUST FILLED TANKS. WATER IN FUEL.   </t>
   </si>
   <si>
-    <t>ENGINE, POWER, TAKEOFF, AIRCRAFT, LANDING, PILOT, TANKS, WATER, FUEL</t>
+    <t>ENGINE; POWER; TAKEOFF; AIRCRAFT; LANDING; PILOT; TANKS; WATER; FUEL</t>
   </si>
   <si>
     <t>19840121015319I</t>
@@ -397,7 +397,7 @@
     <t xml:space="preserve">ENGINE FAILED AFTER TAKEOFF. TRIED TO MAKE A ROAD BUT DRIFTED OFF THE EDGE. FOUND SOLID ICE IN CARBURETOR BOWL.    </t>
   </si>
   <si>
-    <t>ENGINE, TAKEOFF, ROAD, ICE, CARBURETOR BOWL</t>
+    <t>ENGINE; TAKEOFF; ROAD; ICE; CARBURETOR BOWL</t>
   </si>
   <si>
     <t>19950527014439A</t>
@@ -406,7 +406,7 @@
     <t>LOST CONTROL ON CLIMBOUT AFTER TOW RELEASE. ROLLED BOTH WAYS. SPIRAL TO IMPACT. NEGLECTED TO CONNECT RIGHT AILERON.</t>
   </si>
   <si>
-    <t>CLIMBOUT, TOW RELEASE, RIGHT AILERON</t>
+    <t>CLIMBOUT; TOW RELEASE; RIGHT AILERON</t>
   </si>
   <si>
     <t>19960322013629I</t>
@@ -415,7 +415,7 @@
     <t>NARRATIVE: THE AIRCRAFT WAS BEING FERRIED FOR MAINTENANCE. THE GEAR BLOCKED DOWN AND THE NOSE BLOCK FELL OUT DURING</t>
   </si>
   <si>
-    <t>AIRCRAFT, MAINTENANCE, GEAR, NOSE BLOCK</t>
+    <t>AIRCRAFT; MAINTENANCE; GEAR; NOSE BLOCK</t>
   </si>
   <si>
     <t>19960504009509A</t>
@@ -424,7 +424,7 @@
     <t>FAILED TO DETACH TRAILER TIE DOWN FROM SKID. LOST CONTROL AND ROLLED ON LIFT OFF. (-23) PILOT FAILED TO FULLY DETAC</t>
   </si>
   <si>
-    <t>TRAILER, TIE DOWN, SKID, PILOT</t>
+    <t>TRAILER; TIE DOWN; SKID; PILOT</t>
   </si>
   <si>
     <t>19790211002709A</t>
@@ -433,7 +433,7 @@
     <t xml:space="preserve">AIRCRAFT FAILED TO LIFTOFF RUNWAY. RAN OFF END INTO SNOW BANK. FROST ON AIRFRAME.                                  </t>
   </si>
   <si>
-    <t>AIRCRAFT, LIFTOFF, RUNWAY, SNOW BANK, FROST, AIRFRAME</t>
+    <t>AIRCRAFT; LIFTOFF; RUNWAY; SNOW BANK; FROST; AIRFRAME</t>
   </si>
   <si>
     <t>19850418016709I</t>
@@ -442,7 +442,7 @@
     <t xml:space="preserve">ENGINE POWER FAILURE WHILE DOING AEROBATICS. LANDED IN FIELD. PILOT DID NOT VISUALLY INSPECT FUEL TANKS.           </t>
   </si>
   <si>
-    <t>ENGINE, POWER FAILURE, AEROBATICS, FIELD, PILOT, FUEL TANKS</t>
+    <t>ENGINE; POWER FAILURE; AEROBATICS; FIELD; PILOT; FUEL TANKS</t>
   </si>
   <si>
     <t>19780913017419I</t>
@@ -451,7 +451,7 @@
     <t xml:space="preserve">ABORTED TAKEOFF WHEN FRONT BAGGAGE DOOR POPPED OPEN.                                                               </t>
   </si>
   <si>
-    <t>TAKEOFF, BAGGAGE DOOR</t>
+    <t>TAKEOFF; BAGGAGE DOOR</t>
   </si>
   <si>
     <t>19781113027039I</t>
@@ -460,7 +460,7 @@
     <t xml:space="preserve">PILOT TAXIED INTO UNMARKED DITCH AT END OF TAXIWAY.                                                                </t>
   </si>
   <si>
-    <t>PILOT, DITCH, TAXIWAY</t>
+    <t>PILOT; DITCH; TAXIWAY</t>
   </si>
   <si>
     <t>19870606018859A</t>
@@ -469,7 +469,7 @@
     <t xml:space="preserve">UNABLE TO STAY AIRBORNE ON TAKEOFF. ABORTED AND GROUND LOOPED INTO A TREE TO AVOID OVERRUN. MAG SWITCH ON ONE MAG. </t>
   </si>
   <si>
-    <t>TAKEOFF, TREE, MAG SWITCH, ONE MAG</t>
+    <t>TAKEOFF; TREE; MAG SWITCH; ONE MAG</t>
   </si>
   <si>
     <t>19990714022959I</t>
@@ -478,7 +478,7 @@
     <t>(-23) ACCORDING TO THE PILOT HE DEPARTED FRONT RANGE AIRPORT DURING THE HOURS OF DARKNESS. DURING THE START AND RUN</t>
   </si>
   <si>
-    <t>PILOT, FRONT RANGE AIRPORT, HOURS OF DARKNESS, START AND RUN</t>
+    <t>PILOT; FRONT RANGE AIRPORT; HOURS OF DARKNESS; START AND RUN</t>
   </si>
   <si>
     <t>19870319012959I</t>
@@ -487,7 +487,7 @@
     <t xml:space="preserve">NOSE GEAR WOULD NOT RETRACT AFTER TAKEOFF. RETURNED AND FOUND PIN WAS INSTALLED.                                   </t>
   </si>
   <si>
-    <t>TAKEOFF, PIN, NOSE GEAR</t>
+    <t>TAKEOFF; PIN; NOSE GEAR</t>
   </si>
   <si>
     <t>20050504010229A</t>
@@ -496,7 +496,7 @@
     <t xml:space="preserve">(-23) A SIKORSKY S-70A, N160LA, ENCOUNTERED A VIBRATION AFTER THE APU DOOR STRUCK A MAIN ROTOR BLADE INFLIGHT NEAR </t>
   </si>
   <si>
-    <t>SIKORSKY, S-70A, N160LA, VIBRATION, APU DOOR, ROTOR BLADE</t>
+    <t>SIKORSKY; S-70A; N160LA; VIBRATION; APU DOOR; ROTOR BLADE</t>
   </si>
   <si>
     <t>20050429009279I</t>
@@ -505,7 +505,7 @@
     <t>(-23) THE PILOT WAS TAXIING THE AIRCRAFT TO PARKING FOLLOWING A CARGO TRIP. UPON REACHING A POINT WHERE THE TAXIWAY</t>
   </si>
   <si>
-    <t>PILOT, AIRCRAFT, CARGO TRIP, TAXIWAY</t>
+    <t>PILOT; AIRCRAFT; CARGO TRIP; TAXIWAY</t>
   </si>
   <si>
     <t>19890723054159I</t>
@@ -514,7 +514,7 @@
     <t xml:space="preserve">AFTER LANDING IT WAS DETERMINED THERE WAS INSUFFICIENT NUMBER OF SEATS AND OXYGEN MASKS FOR PASSENGERS ONBOARD.    </t>
   </si>
   <si>
-    <t>LANDING, SEATS, OXYGEN MASKS, PASSENGERS</t>
+    <t>LANDING; SEATS; OXYGEN MASKS; PASSENGERS</t>
   </si>
   <si>
     <t>19970523014439I</t>
@@ -523,7 +523,7 @@
     <t>NARRATIVE: THE CARGO DOOR WAS LATCHED BEFORE TAKEOFF BY MR. BOWEN. RUNWAY CONDITIONS AT STEVEN'S VILLAGE WAS EXTREM</t>
   </si>
   <si>
-    <t>CARGO DOOR, TAKEOFF, MR.BOWEN, RUNWAY CONDITIONS, STEVEN'S VILLAGE</t>
+    <t>CARGO DOOR; TAKEOFF; MR.BOWEN; RUNWAY CONDITIONS; STEVEN'S VILLAGE</t>
   </si>
   <si>
     <t>19970908038069A</t>
@@ -532,7 +532,7 @@
     <t xml:space="preserve">TIRED TAXI WITH TIEDOWN CHAINS ATTACHE. ROLLED OVER. PILOT FAILED NOTE RAMP PERSON TIED SKIDS DUE HIGH WIND.       </t>
   </si>
   <si>
-    <t>TIEDOWN CHAINS, PILOT, RAMP PERSON, SKIDS, WIND</t>
+    <t>TIEDOWN CHAINS; PILOT; RAMP PERSON; SKIDS; WIND</t>
   </si>
   <si>
     <t>19781108022239I</t>
@@ -541,7 +541,7 @@
     <t xml:space="preserve">BAGGAGE CART WAS BLOWN INTO PARKED AIRCRAFT BY JET BLAST. BRAKES WERE INOPERATIVE ON CART.                         </t>
   </si>
   <si>
-    <t>BAGGAGE CART, AIRCRAFT, JET BLAST, BRAKES, CART</t>
+    <t>BAGGAGE CART; AIRCRAFT; JET BLAST; BRAKES; CART</t>
   </si>
   <si>
     <t>19760606015529A</t>
@@ -550,7 +550,7 @@
     <t xml:space="preserve">SUFFICIENT OPPORTUNITY EXISTED TO RELEASE WHEN GLIDER ASSUMED NOSE HIGH ATTITUDE.                                  </t>
   </si>
   <si>
-    <t>GLIDER, ALTITUDE</t>
+    <t>GLIDER; ALTITUDE</t>
   </si>
   <si>
     <t>20051009024969I</t>
@@ -559,7 +559,7 @@
     <t>(-23) ^PRIVACY DATA OMITTED^ HELICOPTER ENGINE POWER CHECKS WERE BEING CONDUCTED BY PILOT AND ONE CREWMEMBER. DURIN</t>
   </si>
   <si>
-    <t>HELICOPTER, ENGINE, POWER CHECKS, PILOT, CREWMEMBER</t>
+    <t>HELICOPTER; ENGINE; POWER CHECKS; PILOT; CREWMEMBER</t>
   </si>
   <si>
     <t>19930530020029I</t>
@@ -568,7 +568,7 @@
     <t>PILOT LOST CONTROL OF AIRCRAFT ON TAKEOFF ROLL. PILOTS SEAT WAS NOT LOCKED IN POSITION AND SLID AFT ON ACCELARATION</t>
   </si>
   <si>
-    <t>PILOT, LOST CONTROL, AIRCRAFT, TAKEOFF ROLL, PILOTS, SEAT, POSITION, ACCELERATION</t>
+    <t>PILOT; LOST CONTROL; AIRCRAFT; TAKEOFF ROLL; PILOTS; SEAT; POSITION; ACCELERATION</t>
   </si>
   <si>
     <t>19801230089799I</t>
@@ -577,7 +577,7 @@
     <t>FLAT NOSE STRUT FAILED TO EXTEND BEFORE RETRACTION. IT CAUGHT ON AIRPLANE STRUCTURE, BROKE THE BELLCRANK. COLLAPSED</t>
   </si>
   <si>
-    <t>NOSE STRUT, RETRACTION, AIRPLANE, BELLCRANK</t>
+    <t>NOSE STRUT; RETRACTION; AIRPLANE; BELLCRANK</t>
   </si>
   <si>
     <t>19980508008619A</t>
@@ -586,7 +586,7 @@
     <t>LOST POWER ENROUTE. NOSED OVER LANDING ON A SLOPE. NO EVIDENCE OF FUEL AT SCENE. FAILED TO VISUALLY CHECK FUEL.. (.</t>
   </si>
   <si>
-    <t>POWER, LANDING, SLOPE, EVIDENCE, FUEL, SCENE</t>
+    <t>POWER; LANDING; SLOPE; EVIDENCE; FUEL; SCENE</t>
   </si>
   <si>
     <t>19940818022409A</t>
@@ -595,7 +595,7 @@
     <t>LOST LEFT ENGINE NEAR H71. FEATHERED. HIGH . BEGAN GO AROUND BELOW VMC. CRASHED. BAD OIL LEAK. CRACKED ENGINE CASE.</t>
   </si>
   <si>
-    <t>LEFT ENGINE, H71, VMC, OIL LEAK, ENGINE CASE</t>
+    <t>LEFT ENGINE; H71; VMC; OIL LEAK; ENGINE CASE</t>
   </si>
   <si>
     <t>19920405008919A</t>
@@ -604,7 +604,7 @@
     <t xml:space="preserve">ATTEMPTED TAKEOFF FROM 2500 FT SOD STRIP.GUSTY NORTH WIND,HIT TREES OFF END OF STRIP CRASHED.                      </t>
   </si>
   <si>
-    <t>TAKEOFF, SOD STRIP, NORTH WIND, TREES, STRIP</t>
+    <t>TAKEOFF; SOD STRIP; NORTH WIND; TREES; STRIP</t>
   </si>
   <si>
     <t>19840821046409A</t>
@@ -613,7 +613,7 @@
     <t xml:space="preserve">CRASH OCCURRED DURING FORCED LANDING AFTER ENGINE FAILURE DURING TAKEOFF. AIRCRAFT HAD NOT HAD ANNUAL INSPECTION.  </t>
   </si>
   <si>
-    <t>CRASH, LANDING, ENGINE FAILURE, TAKEOFF, AIRCRAFT, INSPECTION</t>
+    <t>CRASH; LANDING; ENGINE FAILURE; TAKEOFF; AIRCRAFT; INSPECTION</t>
   </si>
   <si>
     <t>19950216008379I</t>
@@ -622,7 +622,7 @@
     <t>NARRATIVE: THE PILOT OF CESSNA 207, N1549U STATED THAT AFTER TAKEOFF FROM THE BETHEL AIRPORT, THE ENGINE STOPPED RU</t>
   </si>
   <si>
-    <t>PILOT, CESSNA 207, N1549U, TAKEOFF, BETHEL AIRPORT, ENGINE</t>
+    <t>PILOT; CESSNA 207; N1549U; TAKEOFF; BETHEL AIRPORT; ENGINE</t>
   </si>
   <si>
     <t>19850525020799A</t>
@@ -631,7 +631,7 @@
     <t xml:space="preserve">TOUCHED DOWN LONG AND BOUNCED. ATTEMPTED DOWNWIND GO AROUND WITH FULL FLAPS. STRUCK TREE 3 MILES FROM AIRPORT.     </t>
   </si>
   <si>
-    <t>FLAPS, TREE, 3 MILES, AIRPORT</t>
+    <t>FLAPS; TREE; 3 MILES; AIRPORT</t>
   </si>
   <si>
     <t>19861114075329I</t>
@@ -640,7 +640,7 @@
     <t xml:space="preserve">ENTERED TCA WITHOUT ATC COMMUNICATION. PILOT WAS AWARE OF MALFUNCTIONING ENCODING ALTIMETER.                       </t>
   </si>
   <si>
-    <t>TCA, ATC COMMUNICATION, PILOT, ALTIMETER</t>
+    <t>TCA; ATC COMMUNICATION; PILOT; ALTIMETER</t>
   </si>
   <si>
     <t>20010421009329I</t>
@@ -649,7 +649,7 @@
     <t>(-23)AIRCRAFT WAS IN CRUISE FLIGHT, THERE WAS A RPM LOSS AND PILOT COULD NOT MAINTAIN ALTITUDE. PILOT MADE AN EMERG</t>
   </si>
   <si>
-    <t>AIRCRAFT, CRUISE FLIGHT, RPM LOSS, PILOT, PILOT, ALTITUDE</t>
+    <t>AIRCRAFT; CRUISE FLIGHT; RPM LOSS; PILOT; PILOT; ALTITUDE</t>
   </si>
   <si>
     <t>19960524045629A</t>
@@ -658,7 +658,7 @@
     <t xml:space="preserve">NOSE BAGGAGE DOOR OPENED ON TAKEOFF. BAGGAGE HIT LEFT PROP. GOT BELWO UMC. LANDED ON SEA ICE. WILL FLY DOOR OPEN.  </t>
   </si>
   <si>
-    <t>NOSE BAGGAGE DOOR, TAKEOFF, BAGGAGE, LEFT PROP, SEA, ICE, DOOR</t>
+    <t>NOSE BAGGAGE DOOR; TAKEOFF; BAGGAGE; LEFT PROP; SEA; ICE; DOOR</t>
   </si>
   <si>
     <t>19871211075169A</t>
@@ -667,7 +667,7 @@
     <t xml:space="preserve">ROUGH ENGINE ON CLIMBOUT. LANDED ON CITY STREET. SPARK PLUGS OUT OF TOLERENCE. FOUND PRIMER UNLOCKED.              </t>
   </si>
   <si>
-    <t>ENGINE, CLIMBOUT, STREET, SPARK PLUGS, TOLERENCE, PRIMER</t>
+    <t>ENGINE; CLIMBOUT; STREET; SPARK PLUGS; TOLERENCE; PRIMER</t>
   </si>
   <si>
     <t>20010910029739I</t>
@@ -676,7 +676,7 @@
     <t>(-23) DURING TAXI OUT, CFI NOTICED NOSE LANDING GEAR GREEN LIGHT WAS OUT. SHE ATTEMPTED TO SWAP LIGHTS TO VERIFY TH</t>
   </si>
   <si>
-    <t>TAXI OUT, CFI,LANDING GEAR, LIGHT, LIGHTS</t>
+    <t>TAXI OUT; CFI;LANDING GEAR; LIGHT; LIGHTS</t>
   </si>
   <si>
     <t>19871027060859A</t>
@@ -685,7 +685,7 @@
     <t>ELECTRIC POWER LOST ON IFR DUAL FLIGHT. STRUCK POWER POLE ON FORCED LANDING, FOUND CIRCUIT BREAKER OFF. PILOT ERROR</t>
   </si>
   <si>
-    <t>POWER, IFR DUAL FLIGHT, POWER POLE, LANDING, CIRCUIT BREAKER, PILOT ERROR</t>
+    <t>POWER; IFR DUAL FLIGHT; POWER POLE; LANDING; CIRCUIT BREAKER; PILOT ERROR</t>
   </si>
   <si>
     <t>19980616023109I</t>
@@ -694,7 +694,7 @@
     <t xml:space="preserve">LOUD BANG AND SHUDDER ENROUTE. SAW SPARKS AT ROTOR. RETURNED. ENGINE COWLING SEPERATED. COWL NOT FASTENED.         </t>
   </si>
   <si>
-    <t>BANG, SHUDDER, SPARKS, ROTOR, COWLING, COWL</t>
+    <t>BANG; SHUDDER; SPARKS; ROTOR; COWLING; COWL</t>
   </si>
   <si>
     <t>19910710026989A</t>
@@ -703,7 +703,7 @@
     <t xml:space="preserve">REPORTED PROBLEM ON CLIMBOUT. STALLED AND CRASHED. NO LOCKING PINS IN SEAT TRACK. SEAT PIN BENT. BELT NOT FASTENED </t>
   </si>
   <si>
-    <t>PROBLEM, CLIMBOUT, LOCKING PINS, SEAT TRACK, SEAT PIN, BELT</t>
+    <t>PROBLEM; CLIMBOUT; LOCKING PINS; SEAT TRACK; SEAT PIN; BELT</t>
   </si>
   <si>
     <t>19780509032859I</t>
@@ -712,7 +712,7 @@
     <t xml:space="preserve">FORCED LANDING AFTER POWER LOSS. FOUND WATER IN FUEL.                                                              </t>
   </si>
   <si>
-    <t>LANDING, POWER LOSS, WATER, FUEL</t>
+    <t>LANDING; POWER LOSS; WATER; FUEL</t>
   </si>
   <si>
     <t>19800506012169A</t>
@@ -721,7 +721,7 @@
     <t xml:space="preserve">LOST CONTROL OF AIRPLANE ON TAKEOFF ROLL. FAILED TO REMOVE AILERON-ELEVATOR LOCK PIN.                              </t>
   </si>
   <si>
-    <t>AIRPLANE, TAKEOFF ROLL, AILERON-ELEVATOR LOCK PIN</t>
+    <t>AIRPLANE; TAKEOFF ROLL; AILERON-ELEVATOR LOCK PIN</t>
   </si>
   <si>
     <t>19791128035159A</t>
@@ -730,7 +730,7 @@
     <t xml:space="preserve">PILOT LANDED TO WAIT OUT RAIN SHOWER. ON CLIMBOUT, ENGINE RAN ROUGH. PILOT LANDED IN FIELD. CLAIMS WATER IN FUEL.  </t>
   </si>
   <si>
-    <t>PILOT, RAIN SHOWER, CLIMBOUT, ENGINE, FIELD, WATER, FUEL</t>
+    <t>PILOT; RAIN SHOWER; CLIMBOUT; ENGINE; FIELD; WATER; FUEL</t>
   </si>
   <si>
     <t>20060621012279A</t>
@@ -739,7 +739,7 @@
     <t>(-23) THE PILOT ^PRIVACY DA^ STATED THAT DURING TAKEOFF (AT ROTATION) HIS SEAT SLID BACK, CAUSING HIM TO OVERROTATE</t>
   </si>
   <si>
-    <t>PILOT, TAKEOFF, SEAT</t>
+    <t>PILOT; TAKEOFF; SEAT</t>
   </si>
   <si>
     <t>19950314029269I</t>
@@ -748,7 +748,7 @@
     <t>NARRATIVE: ON MARCH 14, 1995, N7016M, AN AMATEUR BUILT AIRCRAFT, MADE AN EMERGENCY OFF AIRPORT LANDING NEAR THE BLO</t>
   </si>
   <si>
-    <t>MARCH 14, 1995, N7016M, AIRCRAFT, EMERGENCY OFF AIRPORT LANDING</t>
+    <t>MARCH 14, 1995; N7016M; AIRCRAFT; EMERGENCY OFF AIRPORT LANDING</t>
   </si>
   <si>
     <t>19800804037399A</t>
@@ -757,7 +757,7 @@
     <t xml:space="preserve">EARLY FUEL EXHAUSTION FROM FUEL SIPHONING FROM IMPROPERLY SECURED VENT CAP. OVERSHOT EMERGENCY LANDING AREA.       </t>
   </si>
   <si>
-    <t>FUEL EXHAUSTION, SIPHONING, VENT CAP, EMERGENCY LANDING AREA</t>
+    <t>FUEL EXHAUSTION; SIPHONING; VENT CAP; EMERGENCY LANDING AREA</t>
   </si>
   <si>
     <t>19780402008409I</t>
@@ -766,7 +766,7 @@
     <t xml:space="preserve">TAXIING AIRCRAFT STRUCK PARKED AIRCRAFT. FOUND WORN OUT &amp; INEFFECTIVE BRAKES AS CAUSE.                             </t>
   </si>
   <si>
-    <t>AIRCRAFT, AIRCRAFT, BRAKES</t>
+    <t>AIRCRAFT; AIRCRAFT; BRAKES</t>
   </si>
   <si>
     <t>19890725041869I</t>
@@ -775,7 +775,7 @@
     <t xml:space="preserve">ON ENGINE START PILOTS SEAT WENT TO FULL AFT POSITION. PUSH THROTTLE IN FULL. AIRCRAFT COLLIDED WITH PARKED PLANE. </t>
   </si>
   <si>
-    <t>ENGINE START, PILOTS, SEAT, THROTTLE, AIRCRAFT, PLANE</t>
+    <t>ENGINE START; PILOTS; SEAT; THROTTLE; AIRCRAFT; PLANE</t>
   </si>
   <si>
     <t>19911222062669I</t>
@@ -784,7 +784,7 @@
     <t xml:space="preserve">AFTER LIFTOFF PILOT NOTICED RIGHT FUEL CAP MISSING. ABORTED. LANDED ON SAME RUNWAY. RAN OFF SIDE OF RUNWAY.        </t>
   </si>
   <si>
-    <t>LIFTOFF, PILOT, RIGHT FUEL CAP, RUNWAY, RUNWAY</t>
+    <t>LIFTOFF; PILOT; RIGHT FUEL CAP; RUNWAY; RUNWAY</t>
   </si>
   <si>
     <t>20030607012509A</t>
@@ -793,7 +793,7 @@
     <t>(-23) THE AIRCRAFT DEPARTED BARTLESVILLE MUNICIPAL AIRPORT (BVO) BARTLESVILLE, OK AT 1147 AM LOCAL TIME FOR A LOCAL</t>
   </si>
   <si>
-    <t>AIRCRAFT, BARTLESVILLE MUNICIPAL AIRPORT, BVO, BARTLESVILLE, OK, 1147 AM LOCAL TIME</t>
+    <t>AIRCRAFT; BARTLESVILLE MUNICIPAL AIRPORT; BVO; BARTLESVILLE, OK; 1147 AM LOCAL TIME</t>
   </si>
   <si>
     <t>19801005072789I</t>
@@ -802,7 +802,7 @@
     <t xml:space="preserve">PILOT RAN OFF END OF RUNWAY WHEN REMAINING BRAKE FAILED.                                                           </t>
   </si>
   <si>
-    <t>PILOT, RUNWAY, BRAKE</t>
+    <t>PILOT; RUNWAY; BRAKE</t>
   </si>
   <si>
     <t>19781210024199I</t>
@@ -811,7 +811,7 @@
     <t xml:space="preserve">WHEELS LOCKED UP AFTER SEVERAL TOUCH AND GO LANDINGS DUE TO SNOW PACKED IN THE WHEEL PANTS.                        </t>
   </si>
   <si>
-    <t>WHEELS, LANDINGS, SNOW</t>
+    <t>WHEELS; LANDINGS; SNOW</t>
   </si>
   <si>
     <t>19950804028629A</t>
@@ -820,7 +820,7 @@
     <t>LOST POWER LANDED HARD IN ROUGH WATER. DAMAGED FLOATS AND LONGERON. WATER IN FUEL. MISREAD WATER IN SUMP TO BE FUEL</t>
   </si>
   <si>
-    <t>POWER, WATER, FLOATS, LONGERON, WATER, FUEL, SUMP</t>
+    <t>POWER; WATER; FLOATS; LONGERON; WATER; FUEL; SUMP</t>
   </si>
   <si>
     <t>20040304003309I</t>
@@ -829,7 +829,7 @@
     <t>(-23) AFTER NORMAL TOUCHDOWN THE AIRCRAFT STARTED SLIDING OR HYDROPLANING TOWARD LEFT SIDE OF RUNWAY, AIRCRAFT STRU</t>
   </si>
   <si>
-    <t>TOUCHDOWN, AIRCRAFT, RUNWAY, AIRCRAFT</t>
+    <t>TOUCHDOWN; AIRCRAFT; RUNWAY; AIRCRAFT</t>
   </si>
   <si>
     <t>19780427013859I</t>
@@ -838,7 +838,7 @@
     <t xml:space="preserve">ENGINE COWLING SEPARATED FROM ENGINE IN FLIGHT.                                                                    </t>
   </si>
   <si>
-    <t>COWLING, ENGINE, FLIGHT</t>
+    <t>COWLING; ENGINE; FLIGHT</t>
   </si>
   <si>
     <t>20070202001609A</t>
@@ -847,7 +847,7 @@
     <t>(-23) ON A FLIGHT FROM NOTH PLATTE, NE, TO IOWA CITY, IA, (487 STATUTE MILES) THE AIRCRAFT LOST POWER NEAR GRINNELL</t>
   </si>
   <si>
-    <t>FLIGHT, NOTH PLATTER, NE, IOWA CITY, IA, 487 STATUTE MILES, AIRCRAFT, POWER, GRINNELL</t>
+    <t>FLIGHT; NOTH PLATTER, NE; IOWA CITY, IA; 487 STATUTE MILES; AIRCRAFT; POWER; GRINNELL</t>
   </si>
   <si>
     <t>19780916024019A</t>
@@ -856,7 +856,7 @@
     <t xml:space="preserve">TIE DOWN STRAP ACROSS LEFT SKID CAUGHT ON TRAILER AND TETHERED HEPER.                                              </t>
   </si>
   <si>
-    <t>TIE DOWN STRAP, LEFT SKID, TRAILER</t>
+    <t>TIE DOWN STRAP; LEFT SKID; TRAILER</t>
   </si>
   <si>
     <t>20060718018299I</t>
@@ -865,7 +865,7 @@
     <t>(-23) THE PILOT IN COMMAND (PIC) FAILED TO ENSURE ALL FUEL TANK CAPS WERE SECURELY FASTENED PRIOR TO DEPARTURE. SUB</t>
   </si>
   <si>
-    <t>PILOT IN COMMAND, PIC, FUEL TANK, CAPS, DEPARTURE</t>
+    <t>PILOT IN COMMAND; PIC; FUEL TANK; CAPS; DEPARTURE</t>
   </si>
   <si>
     <t>20040925025079A</t>
@@ -874,7 +874,7 @@
     <t xml:space="preserve">(-23) FUEL CONTAMINATION IN AIRFRAME FUEL FILTER AS WELL AS IN FUEL FILTER AND ENGINE DRIVEN FUEL PUMP FILTER. THE </t>
   </si>
   <si>
-    <t>FUEL CONTAMINATION, AIRFRAME, FUEL FILTER, FUEL FILTER, ENGINE, FUEL PUMP FILTER</t>
+    <t>FUEL CONTAMINATION; AIRFRAME; FUEL FILTER; FUEL FILTER; ENGINE; FUEL PUMP FILTER</t>
   </si>
   <si>
     <t>19961027033759A</t>
@@ -883,7 +883,7 @@
     <t>PRIOR DEMO FLIGHT. CONNECTING ROD BENT BY HYDRO LOCK IN NR5 CYL ON STARTUP. BROKE. HIT COUNTER WT. BROKE PORP SHAFT</t>
   </si>
   <si>
-    <t>DEMO FLIGHT, ROD, HYRDO LOCK, NR5 CYL, STARTUP, COUNTER WT, SHAFT</t>
+    <t>DEMO FLIGHT; ROD; HYRDO LOCK; NR5 CYL; STARTUP; COUNTER WT; SHAFT</t>
   </si>
   <si>
     <t>19870309039779I</t>
@@ -892,7 +892,7 @@
     <t xml:space="preserve">WHILE TAXIING, THE AIRCRAFT STRUCK N106DA WHICH WAS PARKED.  PILOT WAS UNAWARE OF BRAKE PROBLEMS ON THE AIRCRAFT.  </t>
   </si>
   <si>
-    <t>AIRCRAFT, N106DA, PILOT, BRAKE PROBLEMS, AIRCRAFT</t>
+    <t>AIRCRAFT; N106DA; PILOT; BRAKE PROBLEMS; AIRCRAFT</t>
   </si>
   <si>
     <t>20020619014309A</t>
@@ -901,7 +901,7 @@
     <t>(-23) N759TY, CE-182 WAS EN ROUTE FROM HOT SPRINGS, ARKANSAS TO FAYETTEVILLE, TENNESSEE, WHEN THE AIRCRAFT ENGINE Q</t>
   </si>
   <si>
-    <t>N759TY, CE-182, HOT SPRINGS, ARKANSAS, FAYETTEVILLE, TENNESSEE, AIRCRAFT, ENGINE</t>
+    <t>N759TY; CE-182; HOT SPRINGS, ARKANSAS; FAYETTEVILLE, TENNESSEE; AIRCRAFT; ENGINE</t>
   </si>
   <si>
     <t>19951031041599A</t>
@@ -910,7 +910,7 @@
     <t xml:space="preserve">ON CLIMBOUT NOSE BAGGAGE DOOR OPENED. REDUCED POWER. STALLED. ROLLED. DIVED INTO OCEAN. TEST FLIGHT FROM STORAGE.  </t>
   </si>
   <si>
-    <t>CLIMBOUT, NOSE, BAGGAGE DOOR, POWER, OCEAN, TEST FLIGHT, STORAGE</t>
+    <t>CLIMBOUT; NOSE; BAGGAGE DOOR; POWER; OCEAN; TEST FLIGHT; STORAGE</t>
   </si>
   <si>
     <t>19850729066139I</t>
@@ -919,7 +919,7 @@
     <t>ELEVATOR CONTROL JAMMED SHEN HARNESS CAUGHT ON ELEVATOR CABLE. STICK BOOT NOT FASTENED TO FLOOR. LANDED IN A FIELD.</t>
   </si>
   <si>
-    <t>ELEVATOR CONTROL, HARNESS, ELEVATOR CABLE, STICK BOOT, FLOOR, FIELD</t>
+    <t>ELEVATOR CONTROL; HARNESS; ELEVATOR CABLE; STICK BOOT; FLOOR; FIELD</t>
   </si>
   <si>
     <t>19940226003029A</t>
@@ -928,7 +928,7 @@
     <t xml:space="preserve">LOST POWER EN ROUTE. LANDED ON PRIVATE STRIP. NOSED OVER. LEFT FUEL CAP LEAKED. PREVENTED GRAVITY FUEL FLOW.       </t>
   </si>
   <si>
-    <t>POWER, STRIP,LEFT FUEL CAP, GRAVITY FUEL FLOW</t>
+    <t>POWER; STRIP;LEFT FUEL CAP; GRAVITY FUEL FLOW</t>
   </si>
   <si>
     <t>19780111000459A</t>
@@ -937,7 +937,7 @@
     <t xml:space="preserve">ACFT DISPATCHER HARRASSMENT OF PILOT. PILOT FORGOT TO REMOVE TIEDROPE.                                             </t>
   </si>
   <si>
-    <t>ACFT DISPATCHER, PILOT, PILOT</t>
+    <t>ACFT DISPATCHER; PILOT; PILOT</t>
   </si>
   <si>
     <t>20010411006739I</t>
@@ -946,7 +946,7 @@
     <t>(-23) THE HELICOPTER WAS IDLING ON THE HELIPAD, AND THE RPM CONTROL WAS BROUGHT UP TO FLY POSITION FOR THE TAKEOFF.</t>
   </si>
   <si>
-    <t>HELICOPTER, HELIPAD, RPM CONTROL, FLY POSITION, TAKEOFF</t>
+    <t>HELICOPTER; HELIPAD; RPM CONTROL; FLY POSITION; TAKEOFF</t>
   </si>
   <si>
     <t>19870816062719I</t>
@@ -955,7 +955,7 @@
     <t xml:space="preserve">A COPPER TUBE, USED TO HOLD AERIAL BANNERS, FELL THROUGH THE ROOF OF A HOUSE. LOCAL OPERATOR IS BEING MONITORED.   </t>
   </si>
   <si>
-    <t>TUBE, AERIAL BANNERS, ROOF, HOUSE, OPERATOR</t>
+    <t>TUBE; AERIAL BANNERS; ROOF; HOUSE; OPERATOR</t>
   </si>
   <si>
     <t>19980620030289I</t>
@@ -964,7 +964,7 @@
     <t>MR. KADERA THEN ATTEMPTED TO LAND IN A FIELD BUT WAS FORCED TO LAND ON HIGHWAY 93. THREE MILES EAST OF SUNMER, IOWA</t>
   </si>
   <si>
-    <t>MR.KADERA, FIELD, HIGHWAY 93, THREE, EAST, SUNMER, IOWA</t>
+    <t>MR.KADERA; FIELD; HIGHWAY 93; THREE; EAST; SUNMER, IOWA</t>
   </si>
   <si>
     <t>19990923027739A</t>
@@ -973,7 +973,7 @@
     <t>(.19) ON SEPTEMBER 23, 1999, AT 1900 HOURS PACIFIC DAYLIGHT TIME, A HOMEBUILT CIERNIA GLASAIR III, N153JC, EXPERIEN</t>
   </si>
   <si>
-    <t>SEPTEMBER 23,1999, 1900 HOURS PACIFIC DAYLIGHT TIME, CIERNIA GLASAIR III, N153JC</t>
+    <t>SEPTEMBER 23, 1999; 1900 HOURS PACIFIC DAYLIGHT TIME; CIERNIA GLASAIR III; N153JC</t>
   </si>
   <si>
     <t>19980415037339I</t>
@@ -982,7 +982,7 @@
     <t>(-5)NOSE BAGGAGE CARGO CONSISTING OF A WOODEN WHEEL CHOCK SHIFTED DURING FLIGHT AND JAMMED THE NOSE LANDING GEAR ME</t>
   </si>
   <si>
-    <t>NOSE, BAGGAGE, CARGO, WHEEL CHOCK, FLIGHT, NOSE LANDING GEAR</t>
+    <t>NOSE; BAGGAGE; CARGO; WHEEL CHOCK; FLIGHT; NOSE LANDING GEAR</t>
   </si>
   <si>
     <t>19950826026019A</t>
@@ -991,7 +991,7 @@
     <t>EXPLOSION LIFTING LOGS. PITCHED UP, ROLLED. COMPRESSOR STALL NR1 ENGINE. FAILED RELEASE LOGS AND USE SE PROCEDURES.</t>
   </si>
   <si>
-    <t>EXPLOSION, LOGS, COMPRESSOR STALL, NR1 ENGINE, LOGS, SE PROCEDURES</t>
+    <t>EXPLOSION; LOGS; COMPRESSOR STALL; NR1 ENGINE; LOGS; SE PROCEDURES</t>
   </si>
   <si>
     <t>20000215041409A</t>
@@ -1000,7 +1000,7 @@
     <t xml:space="preserve">(.19) ON FEBRUARY 19, 2000, AT 1825 EASTERN STANDARD TIME, A BEECH 1900D, N81SK, OPERATED AS SKYWAY AIRLINE FLIGHT </t>
   </si>
   <si>
-    <t>FEBRUARY 19, 2000, 1825 EASTERN STANDARD TIME, BEECH 1900D, N81SK, SKYWAY AIRLINE, FLIGHT</t>
+    <t>FEBRUARY 19, 2000; 1825 EASTERN STANDARD TIME; BEECH 1900D; N81SK; SKYWAY AIRLINE; FLIGHT</t>
   </si>
   <si>
     <t>19860514036219I</t>
@@ -1009,7 +1009,7 @@
     <t xml:space="preserve">GROUND LOOPED ON LANDING. TAILWHEEL WAS FOUND JAMMED FAR RIGHT.                                                    </t>
   </si>
   <si>
-    <t>GROUND LOOPED, LANDING, TAILWHEEL, RIGHT</t>
+    <t>GROUND LOOPED; LANDING; TAILWHEEL; RIGHT</t>
   </si>
   <si>
     <t>19880527016939A</t>
@@ -1018,7 +1018,7 @@
     <t>ENGINE QUIT ON INITIAL CLIMBOUT. CRASH LANDED AVOIDING TREES. FOUND SELECTED FUEL TANK EMPTY. TRIP WAS TO GET FUEL.</t>
   </si>
   <si>
-    <t>ENGINE, CLIMBOUT, CRASH LANDED, TREES, FUEL TANK, TRIP, FUEL</t>
+    <t>ENGINE; CLIMBOUT; CRASH LANDED; TREES; FUEL TANK; TRIP; FUEL</t>
   </si>
   <si>
     <t>19960418007829A</t>
@@ -1027,7 +1027,7 @@
     <t>CRASHED AND BURNED. (.4)WITNESSES REPORTED THAT AFTER DEPARTURE FROM A GRASS RUNWAY. THE AIRPLANE REACHED AN ALTITU</t>
   </si>
   <si>
-    <t>WITNESSES, DEPARTURE, RUNWAY, AIRPLANE</t>
+    <t>WITNESSES; DEPARTURE; RUNWAY; AIRPLANE</t>
   </si>
   <si>
     <t>19970828026989A</t>
@@ -1036,7 +1036,7 @@
     <t>LOUD POP ON TAKEOFF ROLL. LOST RUDDER CONTROL. EXITED RWY INTO CORNFIELD. HAD FAILED TO LOCK THE TAILWHEEL. (-23) M</t>
   </si>
   <si>
-    <t>POP, TAKEOFF ROLL, LOST RUDDER CONTROL, RWY, CORNFIELD, TAILWHEEL</t>
+    <t>POP; TAKEOFF ROLL; LOST RUDDER CONTROL; RWY; CORNFIELD; TAILWHEEL</t>
   </si>
   <si>
     <t>19870523018729A</t>
@@ -1045,7 +1045,7 @@
     <t xml:space="preserve">CANOPY CAME OPEN ON CLIMBOUT CAUSING AN UNCONTROLLED GROUND COLLISION, NO DEFECTS REPORTED. APPEARS PILOT ERROR.   </t>
   </si>
   <si>
-    <t>CANOPY, CLIMBOUT, GROUND COLLISION, DEFECTS, PILOT ERROR</t>
+    <t>CANOPY; CLIMBOUT; GROUND COLLISION; DEFECTS; PILOT ERROR</t>
   </si>
   <si>
     <t>20030620012809I</t>
@@ -1054,7 +1054,7 @@
     <t xml:space="preserve">(-23) PILOT FAILED TO ASSURE THE OIL FILLER CAP WAS SECURE AND TOOK OFF. OIL WAS OBSERVED COMING OUT OF THE ENGINE </t>
   </si>
   <si>
-    <t>PILOT, OIL FILLER CAP, OIL, ENGINE</t>
+    <t>PILOT; OIL FILLER CAP; OIL; ENGINE</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1129,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1151,14 +1151,20 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1404,7 +1410,7 @@
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1418,7 +1424,7 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1432,7 +1438,7 @@
       <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="8" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1446,7 +1452,7 @@
       <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1460,7 +1466,7 @@
       <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="7" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1474,7 +1480,7 @@
       <c r="C7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1488,7 +1494,7 @@
       <c r="C8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1502,7 +1508,7 @@
       <c r="C9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="7" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1516,7 +1522,7 @@
       <c r="C10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1530,7 +1536,7 @@
       <c r="C11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1544,7 +1550,7 @@
       <c r="C12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="8" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1558,7 +1564,7 @@
       <c r="C13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="9" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1572,7 +1578,7 @@
       <c r="C14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="9" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1586,7 +1592,7 @@
       <c r="C15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1600,7 +1606,7 @@
       <c r="C16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="7" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1614,7 +1620,7 @@
       <c r="C17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="7" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1628,7 +1634,7 @@
       <c r="C18" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="9" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1642,7 +1648,7 @@
       <c r="C19" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="7" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1656,7 +1662,7 @@
       <c r="C20" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="7" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1670,7 +1676,7 @@
       <c r="C21" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="9" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1684,7 +1690,7 @@
       <c r="C22" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="9" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1698,7 +1704,7 @@
       <c r="C23" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="9" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1712,7 +1718,7 @@
       <c r="C24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="9" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1726,7 +1732,7 @@
       <c r="C25" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="7" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1740,7 +1746,7 @@
       <c r="C26" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="10" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1754,7 +1760,7 @@
       <c r="C27" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="8" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1768,7 +1774,7 @@
       <c r="C28" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="9" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1782,7 +1788,7 @@
       <c r="C29" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="7" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1796,7 +1802,7 @@
       <c r="C30" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="9" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1810,7 +1816,7 @@
       <c r="C31" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="9" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1824,7 +1830,7 @@
       <c r="C32" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="7" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1838,7 +1844,7 @@
       <c r="C33" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="9" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1852,7 +1858,7 @@
       <c r="C34" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="9" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1866,7 +1872,7 @@
       <c r="C35" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="9" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1880,7 +1886,7 @@
       <c r="C36" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="7" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1894,7 +1900,7 @@
       <c r="C37" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="7" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1908,7 +1914,7 @@
       <c r="C38" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="9" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1922,7 +1928,7 @@
       <c r="C39" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="7" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1936,7 +1942,7 @@
       <c r="C40" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="9" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1950,7 +1956,7 @@
       <c r="C41" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="9" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1964,7 +1970,7 @@
       <c r="C42" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="9" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1978,7 +1984,7 @@
       <c r="C43" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="7" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1992,7 +1998,7 @@
       <c r="C44" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="9" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2006,7 +2012,7 @@
       <c r="C45" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="7" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2020,7 +2026,7 @@
       <c r="C46" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2034,7 +2040,7 @@
       <c r="C47" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="7" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2048,7 +2054,7 @@
       <c r="C48" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="9" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2062,7 +2068,7 @@
       <c r="C49" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D49" s="7" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2076,7 +2082,7 @@
       <c r="C50" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="D50" s="7" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2090,7 +2096,7 @@
       <c r="C51" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="D51" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2104,7 +2110,7 @@
       <c r="C52" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="9" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2118,7 +2124,7 @@
       <c r="C53" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2132,7 +2138,7 @@
       <c r="C54" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="D54" s="7" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2146,7 +2152,7 @@
       <c r="C55" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="9" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2160,7 +2166,7 @@
       <c r="C56" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D56" s="7" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2174,7 +2180,7 @@
       <c r="C57" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D57" s="7" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2188,7 +2194,7 @@
       <c r="C58" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="D58" s="6" t="s">
+      <c r="D58" s="7" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2202,7 +2208,7 @@
       <c r="C59" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D59" s="7" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2216,7 +2222,7 @@
       <c r="C60" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="D60" s="9" t="s">
+      <c r="D60" s="11" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2230,7 +2236,7 @@
       <c r="C61" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="9" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2244,7 +2250,7 @@
       <c r="C62" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="D62" s="7" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2258,7 +2264,7 @@
       <c r="C63" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="9" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2272,7 +2278,7 @@
       <c r="C64" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="9" t="s">
         <v>192</v>
       </c>
     </row>
@@ -2286,7 +2292,7 @@
       <c r="C65" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D65" s="9" t="s">
         <v>195</v>
       </c>
     </row>
@@ -2300,7 +2306,7 @@
       <c r="C66" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="D66" s="7" t="s">
         <v>198</v>
       </c>
     </row>
@@ -2314,7 +2320,7 @@
       <c r="C67" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D67" s="6" t="s">
+      <c r="D67" s="7" t="s">
         <v>201</v>
       </c>
     </row>
@@ -2328,7 +2334,7 @@
       <c r="C68" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D68" s="9" t="s">
         <v>204</v>
       </c>
     </row>
@@ -2342,7 +2348,7 @@
       <c r="C69" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D69" s="9" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2356,7 +2362,7 @@
       <c r="C70" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D70" s="9" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2370,7 +2376,7 @@
       <c r="C71" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="D71" s="6" t="s">
+      <c r="D71" s="7" t="s">
         <v>213</v>
       </c>
     </row>
@@ -2384,7 +2390,7 @@
       <c r="C72" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D72" s="8" t="s">
+      <c r="D72" s="10" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2398,7 +2404,7 @@
       <c r="C73" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="D73" s="7" t="s">
+      <c r="D73" s="9" t="s">
         <v>219</v>
       </c>
     </row>
@@ -2412,7 +2418,7 @@
       <c r="C74" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="D74" s="7" t="s">
+      <c r="D74" s="9" t="s">
         <v>222</v>
       </c>
     </row>
@@ -2426,7 +2432,7 @@
       <c r="C75" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="D75" s="7" t="s">
+      <c r="D75" s="9" t="s">
         <v>225</v>
       </c>
     </row>
@@ -2440,7 +2446,7 @@
       <c r="C76" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="D76" s="7" t="s">
+      <c r="D76" s="9" t="s">
         <v>228</v>
       </c>
     </row>
@@ -2454,7 +2460,7 @@
       <c r="C77" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D77" s="9" t="s">
         <v>231</v>
       </c>
     </row>
@@ -2468,7 +2474,7 @@
       <c r="C78" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="D78" s="8" t="s">
+      <c r="D78" s="10" t="s">
         <v>234</v>
       </c>
     </row>
@@ -2482,7 +2488,7 @@
       <c r="C79" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="D79" s="6" t="s">
+      <c r="D79" s="7" t="s">
         <v>237</v>
       </c>
     </row>
@@ -2496,7 +2502,7 @@
       <c r="C80" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="D80" s="7" t="s">
+      <c r="D80" s="9" t="s">
         <v>240</v>
       </c>
     </row>
@@ -2510,7 +2516,7 @@
       <c r="C81" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D81" s="8" t="s">
+      <c r="D81" s="10" t="s">
         <v>243</v>
       </c>
     </row>
@@ -2524,7 +2530,7 @@
       <c r="C82" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="D82" s="6" t="s">
+      <c r="D82" s="7" t="s">
         <v>246</v>
       </c>
     </row>
@@ -2538,7 +2544,7 @@
       <c r="C83" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="D83" s="7" t="s">
+      <c r="D83" s="9" t="s">
         <v>249</v>
       </c>
     </row>
@@ -2552,7 +2558,7 @@
       <c r="C84" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="D84" s="9" t="s">
+      <c r="D84" s="10" t="s">
         <v>252</v>
       </c>
     </row>
@@ -2566,7 +2572,7 @@
       <c r="C85" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="D85" s="6" t="s">
+      <c r="D85" s="7" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2580,7 +2586,7 @@
       <c r="C86" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="D86" s="7" t="s">
+      <c r="D86" s="9" t="s">
         <v>258</v>
       </c>
     </row>
@@ -2594,7 +2600,7 @@
       <c r="C87" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="D87" s="6" t="s">
+      <c r="D87" s="7" t="s">
         <v>261</v>
       </c>
     </row>
@@ -2608,7 +2614,7 @@
       <c r="C88" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="D88" s="7" t="s">
+      <c r="D88" s="9" t="s">
         <v>264</v>
       </c>
     </row>
@@ -2622,7 +2628,7 @@
       <c r="C89" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="D89" s="7" t="s">
+      <c r="D89" s="9" t="s">
         <v>267</v>
       </c>
     </row>
@@ -2636,7 +2642,7 @@
       <c r="C90" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="D90" s="7" t="s">
+      <c r="D90" s="9" t="s">
         <v>270</v>
       </c>
     </row>
@@ -2650,7 +2656,7 @@
       <c r="C91" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="D91" s="6" t="s">
+      <c r="D91" s="7" t="s">
         <v>273</v>
       </c>
     </row>
@@ -2664,7 +2670,7 @@
       <c r="C92" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="D92" s="9" t="s">
+      <c r="D92" s="10" t="s">
         <v>276</v>
       </c>
     </row>
@@ -2678,7 +2684,7 @@
       <c r="C93" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="D93" s="5" t="s">
+      <c r="D93" s="8" t="s">
         <v>279</v>
       </c>
     </row>
@@ -2692,7 +2698,7 @@
       <c r="C94" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="D94" s="7" t="s">
+      <c r="D94" s="9" t="s">
         <v>282</v>
       </c>
     </row>
@@ -2706,7 +2712,7 @@
       <c r="C95" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="D95" s="9" t="s">
+      <c r="D95" s="10" t="s">
         <v>285</v>
       </c>
     </row>
@@ -2720,7 +2726,7 @@
       <c r="C96" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="D96" s="6" t="s">
+      <c r="D96" s="7" t="s">
         <v>288</v>
       </c>
     </row>
@@ -2734,7 +2740,7 @@
       <c r="C97" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="D97" s="7" t="s">
+      <c r="D97" s="9" t="s">
         <v>291</v>
       </c>
     </row>
@@ -2748,7 +2754,7 @@
       <c r="C98" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D98" s="7" t="s">
+      <c r="D98" s="9" t="s">
         <v>294</v>
       </c>
     </row>
@@ -2762,7 +2768,7 @@
       <c r="C99" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="D99" s="6" t="s">
+      <c r="D99" s="7" t="s">
         <v>297</v>
       </c>
     </row>
@@ -2776,7 +2782,7 @@
       <c r="C100" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="D100" s="6" t="s">
+      <c r="D100" s="7" t="s">
         <v>300</v>
       </c>
     </row>
@@ -2790,7 +2796,7 @@
       <c r="C101" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="D101" s="7" t="s">
+      <c r="D101" s="9" t="s">
         <v>303</v>
       </c>
     </row>

</xml_diff>